<commit_message>
getting the event view page into place, few other changes as well
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/artifacts.xlsx
+++ b/resources/data-imports/Items/artifacts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
   <si>
     <t>id</t>
   </si>
@@ -261,6 +261,15 @@
   </si>
   <si>
     <t>Eye of the eagle</t>
+  </si>
+  <si>
+    <t>Ancestral Soldiers Statue</t>
+  </si>
+  <si>
+    <t>A simple soldiers statue from a frozen waste land of depsiar and loss. What secrets could this item hold, what lies will it whisper in the icey cold winds?</t>
+  </si>
+  <si>
+    <t>Ice Strength</t>
   </si>
 </sst>
 </file>
@@ -600,7 +609,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BT4"/>
+  <dimension ref="A1:BT5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -926,25 +935,22 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="S2">
         <v>0.5</v>
       </c>
       <c r="U2">
-        <v>0.75</v>
+        <v>0.45</v>
       </c>
       <c r="X2">
-        <v>2</v>
+        <v>0.6</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="AC2">
         <v>1</v>
@@ -964,19 +970,7 @@
       <c r="AM2">
         <v>0</v>
       </c>
-      <c r="AS2">
-        <v>0</v>
-      </c>
       <c r="AV2">
-        <v>0</v>
-      </c>
-      <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="BA2">
         <v>0</v>
       </c>
       <c r="BB2">
@@ -1042,25 +1036,25 @@
         <v>0</v>
       </c>
       <c r="Q3">
+        <v>0.3</v>
+      </c>
+      <c r="R3">
         <v>0.45</v>
       </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
       <c r="S3">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="U3">
-        <v>0.75</v>
+        <v>0.45</v>
       </c>
       <c r="W3">
-        <v>2</v>
+        <v>0.6</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="AC3">
         <v>1</v>
@@ -1080,19 +1074,7 @@
       <c r="AM3">
         <v>0</v>
       </c>
-      <c r="AS3">
-        <v>0</v>
-      </c>
       <c r="AV3">
-        <v>0</v>
-      </c>
-      <c r="AX3">
-        <v>0</v>
-      </c>
-      <c r="AY3">
-        <v>0</v>
-      </c>
-      <c r="BA3">
         <v>0</v>
       </c>
       <c r="BB3">
@@ -1134,7 +1116,7 @@
     </row>
     <row r="4" spans="1:72">
       <c r="A4">
-        <v>1095075</v>
+        <v>1170414</v>
       </c>
       <c r="C4" t="s">
         <v>79</v>
@@ -1146,27 +1128,75 @@
         <v>80</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0.2</v>
+      </c>
+      <c r="R4">
+        <v>0.15</v>
+      </c>
+      <c r="S4">
+        <v>0.1</v>
       </c>
       <c r="U4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="V4">
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>0.6</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
       </c>
       <c r="AC4">
         <v>1</v>
       </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
       <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4">
+        <v>0</v>
+      </c>
+      <c r="BE4">
+        <v>0</v>
+      </c>
+      <c r="BF4">
+        <v>0</v>
+      </c>
+      <c r="BG4">
         <v>0</v>
       </c>
       <c r="BM4">
@@ -1186,6 +1216,59 @@
       </c>
       <c r="BT4" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:72">
+      <c r="A5">
+        <v>2394030</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q5">
+        <v>0.25</v>
+      </c>
+      <c r="S5">
+        <v>0.3</v>
+      </c>
+      <c r="T5">
+        <v>0.4</v>
+      </c>
+      <c r="U5">
+        <v>0.15</v>
+      </c>
+      <c r="V5">
+        <v>0.1</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="BM5">
+        <v>0</v>
+      </c>
+      <c r="BN5">
+        <v>0</v>
+      </c>
+      <c r="BO5">
+        <v>0</v>
+      </c>
+      <c r="BP5">
+        <v>0</v>
+      </c>
+      <c r="BQ5">
+        <v>0</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new ancestral item and its item skills. Minor fix to the skill tree front end.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/artifacts.xlsx
+++ b/resources/data-imports/Items/artifacts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
   <si>
     <t>id</t>
   </si>
@@ -270,6 +270,15 @@
   </si>
   <si>
     <t>Ice Strength</t>
+  </si>
+  <si>
+    <t>Ancestral Fang of Delusional Thougts</t>
+  </si>
+  <si>
+    <t>A fang found in the memories of those deluded by the past. It contains the power of an ancient and yet powerful vampire: Tristie, she ruled the night and brought terror to those who crept through the shadows</t>
+  </si>
+  <si>
+    <t>Twisted Blood Lust</t>
   </si>
 </sst>
 </file>
@@ -609,7 +618,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BT5"/>
+  <dimension ref="A1:BT6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -623,7 +632,7 @@
     <col min="4" max="4" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="238.228" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="245.226" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="19.995" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="15.282" bestFit="true" customWidth="true" style="0"/>
@@ -688,7 +697,7 @@
     <col min="69" max="69" width="22.28" bestFit="true" customWidth="true" style="0"/>
     <col min="70" max="70" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="71" max="71" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="72" max="72" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="72" max="72" width="22.28" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72">
@@ -937,20 +946,23 @@
       <c r="Q2">
         <v>0.3</v>
       </c>
+      <c r="R2">
+        <v>0.25</v>
+      </c>
       <c r="S2">
         <v>0.5</v>
       </c>
       <c r="U2">
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
       <c r="X2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
       <c r="AC2">
         <v>1</v>
@@ -1045,16 +1057,16 @@
         <v>0.25</v>
       </c>
       <c r="U3">
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
       <c r="W3">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
       <c r="AC3">
         <v>1</v>
@@ -1149,13 +1161,13 @@
         <v>0.1</v>
       </c>
       <c r="U4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="V4">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="Y4">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
       <c r="Z4">
         <v>0</v>
@@ -1220,7 +1232,7 @@
     </row>
     <row r="5" spans="1:72">
       <c r="A5">
-        <v>2394030</v>
+        <v>2406742</v>
       </c>
       <c r="C5" t="s">
         <v>82</v>
@@ -1231,6 +1243,9 @@
       <c r="G5" t="s">
         <v>83</v>
       </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
       <c r="Q5">
         <v>0.25</v>
       </c>
@@ -1246,10 +1261,61 @@
       <c r="V5">
         <v>0.1</v>
       </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
       <c r="AC5">
         <v>1</v>
       </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
       <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BD5">
+        <v>0</v>
+      </c>
+      <c r="BE5">
+        <v>0</v>
+      </c>
+      <c r="BF5">
+        <v>0</v>
+      </c>
+      <c r="BG5">
         <v>0</v>
       </c>
       <c r="BM5">
@@ -1269,6 +1335,56 @@
       </c>
       <c r="BT5" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:72">
+      <c r="A6">
+        <v>3301314</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q6">
+        <v>0.5</v>
+      </c>
+      <c r="R6">
+        <v>0.25</v>
+      </c>
+      <c r="S6">
+        <v>0.3</v>
+      </c>
+      <c r="U6">
+        <v>0.4</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="BM6">
+        <v>0</v>
+      </c>
+      <c r="BN6">
+        <v>0</v>
+      </c>
+      <c r="BO6">
+        <v>0</v>
+      </c>
+      <c r="BP6">
+        <v>0</v>
+      </c>
+      <c r="BQ6">
+        <v>0</v>
+      </c>
+      <c r="BT6" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new ancestral item, raid enemies and boss for new labyrinth raid
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/artifacts.xlsx
+++ b/resources/data-imports/Items/artifacts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>Twisted Blood Lust</t>
+  </si>
+  <si>
+    <t>Blacksmiths Anvil</t>
+  </si>
+  <si>
+    <t>A small light weight anvil that glistens with magic. A blacksmith might like this!</t>
+  </si>
+  <si>
+    <t>Enraged Muscles</t>
   </si>
 </sst>
 </file>
@@ -618,7 +627,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BT6"/>
+  <dimension ref="A1:BT7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -982,7 +991,19 @@
       <c r="AM2">
         <v>0</v>
       </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
       <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
         <v>0</v>
       </c>
       <c r="BB2">
@@ -1086,7 +1107,19 @@
       <c r="AM3">
         <v>0</v>
       </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
       <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
         <v>0</v>
       </c>
       <c r="BB3">
@@ -1190,7 +1223,19 @@
       <c r="AM4">
         <v>0</v>
       </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
       <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
         <v>0</v>
       </c>
       <c r="BB4">
@@ -1339,7 +1384,7 @@
     </row>
     <row r="6" spans="1:72">
       <c r="A6">
-        <v>3301314</v>
+        <v>3563363</v>
       </c>
       <c r="C6" t="s">
         <v>85</v>
@@ -1350,6 +1395,9 @@
       <c r="G6" t="s">
         <v>86</v>
       </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
       <c r="Q6">
         <v>0.5</v>
       </c>
@@ -1362,10 +1410,61 @@
       <c r="U6">
         <v>0.4</v>
       </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
       <c r="AC6">
         <v>1</v>
       </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
       <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
+      <c r="BC6">
+        <v>0</v>
+      </c>
+      <c r="BD6">
+        <v>0</v>
+      </c>
+      <c r="BE6">
+        <v>0</v>
+      </c>
+      <c r="BF6">
+        <v>0</v>
+      </c>
+      <c r="BG6">
         <v>0</v>
       </c>
       <c r="BM6">
@@ -1385,6 +1484,62 @@
       </c>
       <c r="BT6" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:72">
+      <c r="A7">
+        <v>4418294</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q7">
+        <v>0.45</v>
+      </c>
+      <c r="R7">
+        <v>0.1</v>
+      </c>
+      <c r="S7">
+        <v>0.3</v>
+      </c>
+      <c r="T7">
+        <v>0.4</v>
+      </c>
+      <c r="U7">
+        <v>0.15</v>
+      </c>
+      <c r="V7">
+        <v>0.1</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="BM7">
+        <v>0</v>
+      </c>
+      <c r="BN7">
+        <v>0</v>
+      </c>
+      <c r="BO7">
+        <v>0</v>
+      </c>
+      <c r="BP7">
+        <v>0</v>
+      </c>
+      <c r="BQ7">
+        <v>0</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>